<commit_message>
Add Problem Set 1 files and supporting literature
Added LaTeX source, output PDF, and figures for Problem Set 1 in ps1/20532_Macroeconometrics___Problem_Set_1. Included helper .tex files and generated output images. Added supporting literature PDFs to the literature directory and updated references. Also updated .DS_Store and Romer_Romer2004.xlsx files.
</commit_message>
<xml_diff>
--- a/ps2/Data/Romer_Romer2004.xlsx
+++ b/ps2/Data/Romer_Romer2004.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefanograziosi/Documents/GitHub/20532-macroeconometrics-ps/ps2/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C77C4C5-521B-DB4A-856E-D21A0971A6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74D252E-8F21-5644-9755-ADBEA33636DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="500" windowWidth="27800" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -380,7 +380,7 @@
   <dimension ref="A1:E157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113"/>
+      <selection activeCell="H113" sqref="H113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>